<commit_message>
add some conditional formatting to see if Bach Ma has lower detection rates than QuangNam and Hue
</commit_message>
<xml_diff>
--- a/analysis/reservecode_by_OTU_samplecount.xlsx
+++ b/analysis/reservecode_by_OTU_samplecount.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Negorashi2011/Downloads/iDNA/Vietnam_leeches/analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{EBCA04E5-6487-C045-B4C9-07602D1E6932}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC0EA18A-88D3-1241-857B-C787A8213CB2}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1380" yWindow="440" windowWidth="30840" windowHeight="23560" activeTab="1"/>
+    <workbookView xWindow="1380" yWindow="440" windowWidth="30840" windowHeight="23560" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="reservecode_by_OTU_samplecount" sheetId="1" r:id="rId1"/>
@@ -243,7 +243,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18">
     <font>
       <sz val="12"/>
@@ -1242,7 +1242,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BE8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2642,14 +2642,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:S59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="4" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="4" topLeftCell="F5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="D22" sqref="D22"/>
+      <selection pane="bottomRight" activeCell="N14" sqref="N14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2828,15 +2828,15 @@
         <v>11</v>
       </c>
       <c r="O3" s="26">
-        <f t="shared" ref="O3:O4" si="2">G3</f>
+        <f t="shared" ref="O3" si="2">G3</f>
         <v>24</v>
       </c>
       <c r="P3" s="26">
-        <f t="shared" ref="P3:P4" si="3">H3</f>
+        <f t="shared" ref="P3" si="3">H3</f>
         <v>160</v>
       </c>
       <c r="Q3" s="27">
-        <f t="shared" ref="Q3:Q4" si="4">I3</f>
+        <f t="shared" ref="Q3" si="4">I3</f>
         <v>189</v>
       </c>
     </row>
@@ -2935,7 +2935,7 @@
         <v>8</v>
       </c>
       <c r="G5" s="3">
-        <f>SUM(E5:F5)</f>
+        <f t="shared" ref="G5:G42" si="12">SUM(E5:F5)</f>
         <v>21</v>
       </c>
       <c r="H5" s="3">
@@ -2945,39 +2945,39 @@
         <v>179</v>
       </c>
       <c r="J5" s="16">
-        <f>B5/B$3</f>
+        <f t="shared" ref="J5:J36" si="13">B5/B$3</f>
         <v>1</v>
       </c>
       <c r="K5" s="16">
-        <f>C5/C$3</f>
+        <f t="shared" ref="K5:K36" si="14">C5/C$3</f>
         <v>0.93650793650793651</v>
       </c>
       <c r="L5" s="16">
-        <f>D5/D$3</f>
+        <f t="shared" ref="L5:L36" si="15">D5/D$3</f>
         <v>0.68918918918918914</v>
       </c>
       <c r="M5" s="16">
-        <f>E5/E$3</f>
+        <f t="shared" ref="M5:M36" si="16">E5/E$3</f>
         <v>1</v>
       </c>
       <c r="N5" s="16">
-        <f>F5/F$3</f>
+        <f t="shared" ref="N5:N36" si="17">F5/F$3</f>
         <v>0.72727272727272729</v>
       </c>
       <c r="O5" s="16">
-        <f>G5/G$3</f>
+        <f t="shared" ref="O5:O36" si="18">G5/G$3</f>
         <v>0.875</v>
       </c>
       <c r="P5" s="16">
-        <f>H5/H$3</f>
+        <f t="shared" ref="P5:P36" si="19">H5/H$3</f>
         <v>0.96250000000000002</v>
       </c>
       <c r="Q5" s="17">
-        <f>I5/I$3</f>
+        <f t="shared" ref="Q5:Q36" si="20">I5/I$3</f>
         <v>0.94708994708994709</v>
       </c>
       <c r="R5" s="15">
-        <f>SUM(B5:I5)</f>
+        <f t="shared" ref="R5:R36" si="21">SUM(B5:I5)</f>
         <v>513</v>
       </c>
     </row>
@@ -3001,7 +3001,7 @@
         <v>4</v>
       </c>
       <c r="G6" s="6">
-        <f>SUM(E6:F6)</f>
+        <f t="shared" si="12"/>
         <v>13</v>
       </c>
       <c r="H6" s="6">
@@ -3011,39 +3011,39 @@
         <v>161</v>
       </c>
       <c r="J6" s="11">
-        <f>B6/B$3</f>
+        <f t="shared" si="13"/>
         <v>0.2857142857142857</v>
       </c>
       <c r="K6" s="11">
-        <f>C6/C$3</f>
+        <f t="shared" si="14"/>
         <v>0.60317460317460314</v>
       </c>
       <c r="L6" s="11">
-        <f>D6/D$3</f>
+        <f t="shared" si="15"/>
         <v>0.56756756756756754</v>
       </c>
       <c r="M6" s="11">
-        <f>E6/E$3</f>
+        <f t="shared" si="16"/>
         <v>0.69230769230769229</v>
       </c>
       <c r="N6" s="11">
-        <f>F6/F$3</f>
+        <f t="shared" si="17"/>
         <v>0.36363636363636365</v>
       </c>
       <c r="O6" s="11">
-        <f>G6/G$3</f>
+        <f t="shared" si="18"/>
         <v>0.54166666666666663</v>
       </c>
       <c r="P6" s="11">
-        <f>H6/H$3</f>
+        <f t="shared" si="19"/>
         <v>0.65625</v>
       </c>
       <c r="Q6" s="12">
-        <f>I6/I$3</f>
+        <f t="shared" si="20"/>
         <v>0.85185185185185186</v>
       </c>
       <c r="R6" s="15">
-        <f>SUM(B6:I6)</f>
+        <f t="shared" si="21"/>
         <v>380</v>
       </c>
     </row>
@@ -3067,7 +3067,7 @@
         <v>4</v>
       </c>
       <c r="G7" s="6">
-        <f>SUM(E7:F7)</f>
+        <f t="shared" si="12"/>
         <v>11</v>
       </c>
       <c r="H7" s="6">
@@ -3077,39 +3077,39 @@
         <v>122</v>
       </c>
       <c r="J7" s="11">
-        <f>B7/B$3</f>
+        <f t="shared" si="13"/>
         <v>0.5357142857142857</v>
       </c>
       <c r="K7" s="11">
-        <f>C7/C$3</f>
+        <f t="shared" si="14"/>
         <v>0.22222222222222221</v>
       </c>
       <c r="L7" s="11">
-        <f>D7/D$3</f>
+        <f t="shared" si="15"/>
         <v>0.6216216216216216</v>
       </c>
       <c r="M7" s="11">
-        <f>E7/E$3</f>
+        <f t="shared" si="16"/>
         <v>0.53846153846153844</v>
       </c>
       <c r="N7" s="11">
-        <f>F7/F$3</f>
+        <f t="shared" si="17"/>
         <v>0.36363636363636365</v>
       </c>
       <c r="O7" s="11">
-        <f>G7/G$3</f>
+        <f t="shared" si="18"/>
         <v>0.45833333333333331</v>
       </c>
       <c r="P7" s="11">
-        <f>H7/H$3</f>
+        <f t="shared" si="19"/>
         <v>0.73124999999999996</v>
       </c>
       <c r="Q7" s="12">
-        <f>I7/I$3</f>
+        <f t="shared" si="20"/>
         <v>0.64550264550264547</v>
       </c>
       <c r="R7" s="15">
-        <f>SUM(B7:I7)</f>
+        <f t="shared" si="21"/>
         <v>336</v>
       </c>
     </row>
@@ -3133,7 +3133,7 @@
         <v>8</v>
       </c>
       <c r="G8" s="6">
-        <f>SUM(E8:F8)</f>
+        <f t="shared" si="12"/>
         <v>17</v>
       </c>
       <c r="H8" s="6">
@@ -3143,39 +3143,39 @@
         <v>152</v>
       </c>
       <c r="J8" s="11">
-        <f>B8/B$3</f>
+        <f t="shared" si="13"/>
         <v>0.17857142857142858</v>
       </c>
       <c r="K8" s="11">
-        <f>C8/C$3</f>
+        <f t="shared" si="14"/>
         <v>6.3492063492063489E-2</v>
       </c>
       <c r="L8" s="11">
-        <f>D8/D$3</f>
+        <f t="shared" si="15"/>
         <v>0.58108108108108103</v>
       </c>
       <c r="M8" s="11">
-        <f>E8/E$3</f>
+        <f t="shared" si="16"/>
         <v>0.69230769230769229</v>
       </c>
       <c r="N8" s="11">
-        <f>F8/F$3</f>
+        <f t="shared" si="17"/>
         <v>0.72727272727272729</v>
       </c>
       <c r="O8" s="11">
-        <f>G8/G$3</f>
+        <f t="shared" si="18"/>
         <v>0.70833333333333337</v>
       </c>
       <c r="P8" s="11">
-        <f>H8/H$3</f>
+        <f t="shared" si="19"/>
         <v>0.31874999999999998</v>
       </c>
       <c r="Q8" s="12">
-        <f>I8/I$3</f>
+        <f t="shared" si="20"/>
         <v>0.80423280423280419</v>
       </c>
       <c r="R8" s="15">
-        <f>SUM(B8:I8)</f>
+        <f t="shared" si="21"/>
         <v>289</v>
       </c>
     </row>
@@ -3199,7 +3199,7 @@
         <v>6</v>
       </c>
       <c r="G9" s="6">
-        <f>SUM(E9:F9)</f>
+        <f t="shared" si="12"/>
         <v>17</v>
       </c>
       <c r="H9" s="6">
@@ -3209,39 +3209,39 @@
         <v>112</v>
       </c>
       <c r="J9" s="11">
-        <f>B9/B$3</f>
+        <f t="shared" si="13"/>
         <v>7.1428571428571425E-2</v>
       </c>
       <c r="K9" s="11">
-        <f>C9/C$3</f>
+        <f t="shared" si="14"/>
         <v>0.58730158730158732</v>
       </c>
       <c r="L9" s="11">
-        <f>D9/D$3</f>
+        <f t="shared" si="15"/>
         <v>0.59459459459459463</v>
       </c>
       <c r="M9" s="11">
-        <f>E9/E$3</f>
+        <f t="shared" si="16"/>
         <v>0.84615384615384615</v>
       </c>
       <c r="N9" s="11">
-        <f>F9/F$3</f>
+        <f t="shared" si="17"/>
         <v>0.54545454545454541</v>
       </c>
       <c r="O9" s="11">
-        <f>G9/G$3</f>
+        <f t="shared" si="18"/>
         <v>0.70833333333333337</v>
       </c>
       <c r="P9" s="11">
-        <f>H9/H$3</f>
+        <f t="shared" si="19"/>
         <v>0.32500000000000001</v>
       </c>
       <c r="Q9" s="12">
-        <f>I9/I$3</f>
+        <f t="shared" si="20"/>
         <v>0.59259259259259256</v>
       </c>
       <c r="R9" s="15">
-        <f>SUM(B9:I9)</f>
+        <f t="shared" si="21"/>
         <v>281</v>
       </c>
     </row>
@@ -3265,7 +3265,7 @@
         <v>2</v>
       </c>
       <c r="G10" s="6">
-        <f>SUM(E10:F10)</f>
+        <f t="shared" si="12"/>
         <v>10</v>
       </c>
       <c r="H10" s="6">
@@ -3275,39 +3275,39 @@
         <v>118</v>
       </c>
       <c r="J10" s="11">
-        <f>B10/B$3</f>
+        <f t="shared" si="13"/>
         <v>0.7142857142857143</v>
       </c>
       <c r="K10" s="11">
-        <f>C10/C$3</f>
+        <f t="shared" si="14"/>
         <v>0.23809523809523808</v>
       </c>
       <c r="L10" s="11">
-        <f>D10/D$3</f>
+        <f t="shared" si="15"/>
         <v>0.17567567567567569</v>
       </c>
       <c r="M10" s="11">
-        <f>E10/E$3</f>
+        <f t="shared" si="16"/>
         <v>0.61538461538461542</v>
       </c>
       <c r="N10" s="11">
-        <f>F10/F$3</f>
+        <f t="shared" si="17"/>
         <v>0.18181818181818182</v>
       </c>
       <c r="O10" s="11">
-        <f>G10/G$3</f>
+        <f t="shared" si="18"/>
         <v>0.41666666666666669</v>
       </c>
       <c r="P10" s="11">
-        <f>H10/H$3</f>
+        <f t="shared" si="19"/>
         <v>0.35625000000000001</v>
       </c>
       <c r="Q10" s="12">
-        <f>I10/I$3</f>
+        <f t="shared" si="20"/>
         <v>0.6243386243386243</v>
       </c>
       <c r="R10" s="15">
-        <f>SUM(B10:I10)</f>
+        <f t="shared" si="21"/>
         <v>243</v>
       </c>
     </row>
@@ -3331,7 +3331,7 @@
         <v>7</v>
       </c>
       <c r="G11" s="30">
-        <f>SUM(E11:F11)</f>
+        <f t="shared" si="12"/>
         <v>13</v>
       </c>
       <c r="H11" s="30">
@@ -3341,39 +3341,39 @@
         <v>45</v>
       </c>
       <c r="J11" s="33">
-        <f>B11/B$3</f>
+        <f t="shared" si="13"/>
         <v>0.39285714285714285</v>
       </c>
       <c r="K11" s="33">
-        <f>C11/C$3</f>
+        <f t="shared" si="14"/>
         <v>0.69841269841269837</v>
       </c>
       <c r="L11" s="33">
-        <f>D11/D$3</f>
+        <f t="shared" si="15"/>
         <v>0.3108108108108108</v>
       </c>
       <c r="M11" s="33">
-        <f>E11/E$3</f>
+        <f t="shared" si="16"/>
         <v>0.46153846153846156</v>
       </c>
       <c r="N11" s="33">
-        <f>F11/F$3</f>
+        <f t="shared" si="17"/>
         <v>0.63636363636363635</v>
       </c>
       <c r="O11" s="33">
-        <f>G11/G$3</f>
+        <f t="shared" si="18"/>
         <v>0.54166666666666663</v>
       </c>
       <c r="P11" s="33">
-        <f>H11/H$3</f>
+        <f t="shared" si="19"/>
         <v>0.46250000000000002</v>
       </c>
       <c r="Q11" s="34">
-        <f>I11/I$3</f>
+        <f t="shared" si="20"/>
         <v>0.23809523809523808</v>
       </c>
       <c r="R11" s="35">
-        <f>SUM(B11:I11)</f>
+        <f t="shared" si="21"/>
         <v>223</v>
       </c>
     </row>
@@ -3397,7 +3397,7 @@
         <v>3</v>
       </c>
       <c r="G12" s="6">
-        <f>SUM(E12:F12)</f>
+        <f t="shared" si="12"/>
         <v>6</v>
       </c>
       <c r="H12" s="6">
@@ -3407,39 +3407,39 @@
         <v>85</v>
       </c>
       <c r="J12" s="11">
-        <f>B12/B$3</f>
+        <f t="shared" si="13"/>
         <v>0.7142857142857143</v>
       </c>
       <c r="K12" s="11">
-        <f>C12/C$3</f>
+        <f t="shared" si="14"/>
         <v>0.20634920634920634</v>
       </c>
       <c r="L12" s="11">
-        <f>D12/D$3</f>
+        <f t="shared" si="15"/>
         <v>0.24324324324324326</v>
       </c>
       <c r="M12" s="11">
-        <f>E12/E$3</f>
+        <f t="shared" si="16"/>
         <v>0.23076923076923078</v>
       </c>
       <c r="N12" s="11">
-        <f>F12/F$3</f>
+        <f t="shared" si="17"/>
         <v>0.27272727272727271</v>
       </c>
       <c r="O12" s="11">
-        <f>G12/G$3</f>
+        <f t="shared" si="18"/>
         <v>0.25</v>
       </c>
       <c r="P12" s="11">
-        <f>H12/H$3</f>
+        <f t="shared" si="19"/>
         <v>0.45</v>
       </c>
       <c r="Q12" s="11">
-        <f>I12/I$3</f>
+        <f t="shared" si="20"/>
         <v>0.44973544973544971</v>
       </c>
       <c r="R12" s="15">
-        <f>SUM(B12:I12)</f>
+        <f t="shared" si="21"/>
         <v>220</v>
       </c>
     </row>
@@ -3463,7 +3463,7 @@
         <v>1</v>
       </c>
       <c r="G13" s="6">
-        <f>SUM(E13:F13)</f>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
       <c r="H13" s="6">
@@ -3473,39 +3473,39 @@
         <v>87</v>
       </c>
       <c r="J13" s="11">
-        <f>B13/B$3</f>
+        <f t="shared" si="13"/>
         <v>0.7857142857142857</v>
       </c>
       <c r="K13" s="11">
-        <f>C13/C$3</f>
+        <f t="shared" si="14"/>
         <v>0.31746031746031744</v>
       </c>
       <c r="L13" s="11">
-        <f>D13/D$3</f>
+        <f t="shared" si="15"/>
         <v>5.4054054054054057E-2</v>
       </c>
       <c r="M13" s="11">
-        <f>E13/E$3</f>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="N13" s="11">
-        <f>F13/F$3</f>
+        <f t="shared" si="17"/>
         <v>9.0909090909090912E-2</v>
       </c>
       <c r="O13" s="11">
-        <f>G13/G$3</f>
+        <f t="shared" si="18"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="P13" s="11">
-        <f>H13/H$3</f>
+        <f t="shared" si="19"/>
         <v>0.38750000000000001</v>
       </c>
       <c r="Q13" s="12">
-        <f>I13/I$3</f>
+        <f t="shared" si="20"/>
         <v>0.46031746031746029</v>
       </c>
       <c r="R13" s="15">
-        <f>SUM(B13:I13)</f>
+        <f t="shared" si="21"/>
         <v>197</v>
       </c>
     </row>
@@ -3529,7 +3529,7 @@
         <v>4</v>
       </c>
       <c r="G14" s="6">
-        <f>SUM(E14:F14)</f>
+        <f t="shared" si="12"/>
         <v>8</v>
       </c>
       <c r="H14" s="6">
@@ -3539,39 +3539,39 @@
         <v>77</v>
       </c>
       <c r="J14" s="11">
-        <f>B14/B$3</f>
+        <f t="shared" si="13"/>
         <v>0.21428571428571427</v>
       </c>
       <c r="K14" s="11">
-        <f>C14/C$3</f>
+        <f t="shared" si="14"/>
         <v>0.25396825396825395</v>
       </c>
       <c r="L14" s="11">
-        <f>D14/D$3</f>
+        <f t="shared" si="15"/>
         <v>0.20270270270270271</v>
       </c>
       <c r="M14" s="11">
-        <f>E14/E$3</f>
+        <f t="shared" si="16"/>
         <v>0.30769230769230771</v>
       </c>
       <c r="N14" s="11">
-        <f>F14/F$3</f>
+        <f t="shared" si="17"/>
         <v>0.36363636363636365</v>
       </c>
       <c r="O14" s="11">
-        <f>G14/G$3</f>
+        <f t="shared" si="18"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="P14" s="11">
-        <f>H14/H$3</f>
+        <f t="shared" si="19"/>
         <v>0.41875000000000001</v>
       </c>
       <c r="Q14" s="12">
-        <f>I14/I$3</f>
+        <f t="shared" si="20"/>
         <v>0.40740740740740738</v>
       </c>
       <c r="R14" s="15">
-        <f>SUM(B14:I14)</f>
+        <f t="shared" si="21"/>
         <v>197</v>
       </c>
     </row>
@@ -3595,7 +3595,7 @@
         <v>3</v>
       </c>
       <c r="G15" s="6">
-        <f>SUM(E15:F15)</f>
+        <f t="shared" si="12"/>
         <v>7</v>
       </c>
       <c r="H15" s="6">
@@ -3605,39 +3605,39 @@
         <v>90</v>
       </c>
       <c r="J15" s="11">
-        <f>B15/B$3</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="K15" s="11">
-        <f>C15/C$3</f>
+        <f t="shared" si="14"/>
         <v>0.22222222222222221</v>
       </c>
       <c r="L15" s="11">
-        <f>D15/D$3</f>
+        <f t="shared" si="15"/>
         <v>0.36486486486486486</v>
       </c>
       <c r="M15" s="11">
-        <f>E15/E$3</f>
+        <f t="shared" si="16"/>
         <v>0.30769230769230771</v>
       </c>
       <c r="N15" s="11">
-        <f>F15/F$3</f>
+        <f t="shared" si="17"/>
         <v>0.27272727272727271</v>
       </c>
       <c r="O15" s="11">
-        <f>G15/G$3</f>
+        <f t="shared" si="18"/>
         <v>0.29166666666666669</v>
       </c>
       <c r="P15" s="11">
-        <f>H15/H$3</f>
+        <f t="shared" si="19"/>
         <v>0.30625000000000002</v>
       </c>
       <c r="Q15" s="12">
-        <f>I15/I$3</f>
+        <f t="shared" si="20"/>
         <v>0.47619047619047616</v>
       </c>
       <c r="R15" s="15">
-        <f>SUM(B15:I15)</f>
+        <f t="shared" si="21"/>
         <v>194</v>
       </c>
     </row>
@@ -3661,7 +3661,7 @@
         <v>1</v>
       </c>
       <c r="G16" s="6">
-        <f>SUM(E16:F16)</f>
+        <f t="shared" si="12"/>
         <v>4</v>
       </c>
       <c r="H16" s="6">
@@ -3671,39 +3671,39 @@
         <v>81</v>
       </c>
       <c r="J16" s="11">
-        <f>B16/B$3</f>
+        <f t="shared" si="13"/>
         <v>0.32142857142857145</v>
       </c>
       <c r="K16" s="11">
-        <f>C16/C$3</f>
+        <f t="shared" si="14"/>
         <v>0.41269841269841268</v>
       </c>
       <c r="L16" s="11">
-        <f>D16/D$3</f>
+        <f t="shared" si="15"/>
         <v>0.20270270270270271</v>
       </c>
       <c r="M16" s="11">
-        <f>E16/E$3</f>
+        <f t="shared" si="16"/>
         <v>0.23076923076923078</v>
       </c>
       <c r="N16" s="11">
-        <f>F16/F$3</f>
+        <f t="shared" si="17"/>
         <v>9.0909090909090912E-2</v>
       </c>
       <c r="O16" s="11">
-        <f>G16/G$3</f>
+        <f t="shared" si="18"/>
         <v>0.16666666666666666</v>
       </c>
       <c r="P16" s="11">
-        <f>H16/H$3</f>
+        <f t="shared" si="19"/>
         <v>0.3</v>
       </c>
       <c r="Q16" s="12">
-        <f>I16/I$3</f>
+        <f t="shared" si="20"/>
         <v>0.42857142857142855</v>
       </c>
       <c r="R16" s="15">
-        <f>SUM(B16:I16)</f>
+        <f t="shared" si="21"/>
         <v>187</v>
       </c>
     </row>
@@ -3727,7 +3727,7 @@
         <v>3</v>
       </c>
       <c r="G17" s="6">
-        <f>SUM(E17:F17)</f>
+        <f t="shared" si="12"/>
         <v>11</v>
       </c>
       <c r="H17" s="6">
@@ -3737,39 +3737,39 @@
         <v>58</v>
       </c>
       <c r="J17" s="11">
-        <f>B17/B$3</f>
+        <f t="shared" si="13"/>
         <v>7.1428571428571425E-2</v>
       </c>
       <c r="K17" s="11">
-        <f>C17/C$3</f>
+        <f t="shared" si="14"/>
         <v>7.9365079365079361E-2</v>
       </c>
       <c r="L17" s="11">
-        <f>D17/D$3</f>
+        <f t="shared" si="15"/>
         <v>0.24324324324324326</v>
       </c>
       <c r="M17" s="11">
-        <f>E17/E$3</f>
+        <f t="shared" si="16"/>
         <v>0.61538461538461542</v>
       </c>
       <c r="N17" s="11">
-        <f>F17/F$3</f>
+        <f t="shared" si="17"/>
         <v>0.27272727272727271</v>
       </c>
       <c r="O17" s="11">
-        <f>G17/G$3</f>
+        <f t="shared" si="18"/>
         <v>0.45833333333333331</v>
       </c>
       <c r="P17" s="11">
-        <f>H17/H$3</f>
+        <f t="shared" si="19"/>
         <v>0.47499999999999998</v>
       </c>
       <c r="Q17" s="12">
-        <f>I17/I$3</f>
+        <f t="shared" si="20"/>
         <v>0.30687830687830686</v>
       </c>
       <c r="R17" s="15">
-        <f>SUM(B17:I17)</f>
+        <f t="shared" si="21"/>
         <v>181</v>
       </c>
     </row>
@@ -3793,7 +3793,7 @@
         <v>0</v>
       </c>
       <c r="G18" s="6">
-        <f>SUM(E18:F18)</f>
+        <f t="shared" si="12"/>
         <v>4</v>
       </c>
       <c r="H18" s="6">
@@ -3803,39 +3803,39 @@
         <v>109</v>
       </c>
       <c r="J18" s="11">
-        <f>B18/B$3</f>
+        <f t="shared" si="13"/>
         <v>0.10714285714285714</v>
       </c>
       <c r="K18" s="11">
-        <f>C18/C$3</f>
+        <f t="shared" si="14"/>
         <v>0.14285714285714285</v>
       </c>
       <c r="L18" s="11">
-        <f>D18/D$3</f>
+        <f t="shared" si="15"/>
         <v>0.24324324324324326</v>
       </c>
       <c r="M18" s="11">
-        <f>E18/E$3</f>
+        <f t="shared" si="16"/>
         <v>0.30769230769230771</v>
       </c>
       <c r="N18" s="11">
-        <f>F18/F$3</f>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="O18" s="11">
-        <f>G18/G$3</f>
+        <f t="shared" si="18"/>
         <v>0.16666666666666666</v>
       </c>
       <c r="P18" s="11">
-        <f>H18/H$3</f>
+        <f t="shared" si="19"/>
         <v>0.1875</v>
       </c>
       <c r="Q18" s="12">
-        <f>I18/I$3</f>
+        <f t="shared" si="20"/>
         <v>0.57671957671957674</v>
       </c>
       <c r="R18" s="15">
-        <f>SUM(B18:I18)</f>
+        <f t="shared" si="21"/>
         <v>177</v>
       </c>
     </row>
@@ -3859,7 +3859,7 @@
         <v>5</v>
       </c>
       <c r="G19" s="6">
-        <f>SUM(E19:F19)</f>
+        <f t="shared" si="12"/>
         <v>11</v>
       </c>
       <c r="H19" s="6">
@@ -3869,39 +3869,39 @@
         <v>44</v>
       </c>
       <c r="J19" s="11">
-        <f>B19/B$3</f>
+        <f t="shared" si="13"/>
         <v>0.17857142857142858</v>
       </c>
       <c r="K19" s="11">
-        <f>C19/C$3</f>
+        <f t="shared" si="14"/>
         <v>0.19047619047619047</v>
       </c>
       <c r="L19" s="11">
-        <f>D19/D$3</f>
+        <f t="shared" si="15"/>
         <v>6.7567567567567571E-2</v>
       </c>
       <c r="M19" s="11">
-        <f>E19/E$3</f>
+        <f t="shared" si="16"/>
         <v>0.46153846153846156</v>
       </c>
       <c r="N19" s="11">
-        <f>F19/F$3</f>
+        <f t="shared" si="17"/>
         <v>0.45454545454545453</v>
       </c>
       <c r="O19" s="11">
-        <f>G19/G$3</f>
+        <f t="shared" si="18"/>
         <v>0.45833333333333331</v>
       </c>
       <c r="P19" s="11">
-        <f>H19/H$3</f>
+        <f t="shared" si="19"/>
         <v>0.35</v>
       </c>
       <c r="Q19" s="12">
-        <f>I19/I$3</f>
+        <f t="shared" si="20"/>
         <v>0.23280423280423279</v>
       </c>
       <c r="R19" s="15">
-        <f>SUM(B19:I19)</f>
+        <f t="shared" si="21"/>
         <v>144</v>
       </c>
     </row>
@@ -3925,7 +3925,7 @@
         <v>0</v>
       </c>
       <c r="G20" s="6">
-        <f>SUM(E20:F20)</f>
+        <f t="shared" si="12"/>
         <v>4</v>
       </c>
       <c r="H20" s="6">
@@ -3935,39 +3935,39 @@
         <v>66</v>
       </c>
       <c r="J20" s="11">
-        <f>B20/B$3</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="K20" s="11">
-        <f>C20/C$3</f>
+        <f t="shared" si="14"/>
         <v>0.20634920634920634</v>
       </c>
       <c r="L20" s="11">
-        <f>D20/D$3</f>
+        <f t="shared" si="15"/>
         <v>0.20270270270270271</v>
       </c>
       <c r="M20" s="11">
-        <f>E20/E$3</f>
+        <f t="shared" si="16"/>
         <v>0.30769230769230771</v>
       </c>
       <c r="N20" s="11">
-        <f>F20/F$3</f>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="O20" s="11">
-        <f>G20/G$3</f>
+        <f t="shared" si="18"/>
         <v>0.16666666666666666</v>
       </c>
       <c r="P20" s="11">
-        <f>H20/H$3</f>
+        <f t="shared" si="19"/>
         <v>8.7499999999999994E-2</v>
       </c>
       <c r="Q20" s="12">
-        <f>I20/I$3</f>
+        <f t="shared" si="20"/>
         <v>0.34920634920634919</v>
       </c>
       <c r="R20" s="15">
-        <f>SUM(B20:I20)</f>
+        <f t="shared" si="21"/>
         <v>116</v>
       </c>
     </row>
@@ -3991,7 +3991,7 @@
         <v>3</v>
       </c>
       <c r="G21" s="6">
-        <f>SUM(E21:F21)</f>
+        <f t="shared" si="12"/>
         <v>8</v>
       </c>
       <c r="H21" s="6">
@@ -4001,39 +4001,39 @@
         <v>34</v>
       </c>
       <c r="J21" s="11">
-        <f>B21/B$3</f>
+        <f t="shared" si="13"/>
         <v>0.14285714285714285</v>
       </c>
       <c r="K21" s="11">
-        <f>C21/C$3</f>
+        <f t="shared" si="14"/>
         <v>0.1111111111111111</v>
       </c>
       <c r="L21" s="11">
-        <f>D21/D$3</f>
+        <f t="shared" si="15"/>
         <v>5.4054054054054057E-2</v>
       </c>
       <c r="M21" s="11">
-        <f>E21/E$3</f>
+        <f t="shared" si="16"/>
         <v>0.38461538461538464</v>
       </c>
       <c r="N21" s="11">
-        <f>F21/F$3</f>
+        <f t="shared" si="17"/>
         <v>0.27272727272727271</v>
       </c>
       <c r="O21" s="11">
-        <f>G21/G$3</f>
+        <f t="shared" si="18"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="P21" s="11">
-        <f>H21/H$3</f>
+        <f t="shared" si="19"/>
         <v>0.20624999999999999</v>
       </c>
       <c r="Q21" s="12">
-        <f>I21/I$3</f>
+        <f t="shared" si="20"/>
         <v>0.17989417989417988</v>
       </c>
       <c r="R21" s="15">
-        <f>SUM(B21:I21)</f>
+        <f t="shared" si="21"/>
         <v>98</v>
       </c>
     </row>
@@ -4057,7 +4057,7 @@
         <v>1</v>
       </c>
       <c r="G22" s="6">
-        <f>SUM(E22:F22)</f>
+        <f t="shared" si="12"/>
         <v>2</v>
       </c>
       <c r="H22" s="6">
@@ -4067,39 +4067,39 @@
         <v>32</v>
       </c>
       <c r="J22" s="11">
-        <f>B22/B$3</f>
+        <f t="shared" si="13"/>
         <v>3.5714285714285712E-2</v>
       </c>
       <c r="K22" s="11">
-        <f>C22/C$3</f>
+        <f t="shared" si="14"/>
         <v>0.58730158730158732</v>
       </c>
       <c r="L22" s="11">
-        <f>D22/D$3</f>
+        <f t="shared" si="15"/>
         <v>4.0540540540540543E-2</v>
       </c>
       <c r="M22" s="11">
-        <f>E22/E$3</f>
+        <f t="shared" si="16"/>
         <v>7.6923076923076927E-2</v>
       </c>
       <c r="N22" s="11">
-        <f>F22/F$3</f>
+        <f t="shared" si="17"/>
         <v>9.0909090909090912E-2</v>
       </c>
       <c r="O22" s="11">
-        <f>G22/G$3</f>
+        <f t="shared" si="18"/>
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="P22" s="11">
-        <f>H22/H$3</f>
+        <f t="shared" si="19"/>
         <v>4.3749999999999997E-2</v>
       </c>
       <c r="Q22" s="12">
-        <f>I22/I$3</f>
+        <f t="shared" si="20"/>
         <v>0.1693121693121693</v>
       </c>
       <c r="R22" s="15">
-        <f>SUM(B22:I22)</f>
+        <f t="shared" si="21"/>
         <v>84</v>
       </c>
     </row>
@@ -4123,7 +4123,7 @@
         <v>4</v>
       </c>
       <c r="G23" s="6">
-        <f>SUM(E23:F23)</f>
+        <f t="shared" si="12"/>
         <v>7</v>
       </c>
       <c r="H23" s="6">
@@ -4133,39 +4133,39 @@
         <v>34</v>
       </c>
       <c r="J23" s="11">
-        <f>B23/B$3</f>
+        <f t="shared" si="13"/>
         <v>7.1428571428571425E-2</v>
       </c>
       <c r="K23" s="11">
-        <f>C23/C$3</f>
+        <f t="shared" si="14"/>
         <v>3.1746031746031744E-2</v>
       </c>
       <c r="L23" s="11">
-        <f>D23/D$3</f>
+        <f t="shared" si="15"/>
         <v>9.45945945945946E-2</v>
       </c>
       <c r="M23" s="11">
-        <f>E23/E$3</f>
+        <f t="shared" si="16"/>
         <v>0.23076923076923078</v>
       </c>
       <c r="N23" s="11">
-        <f>F23/F$3</f>
+        <f t="shared" si="17"/>
         <v>0.36363636363636365</v>
       </c>
       <c r="O23" s="11">
-        <f>G23/G$3</f>
+        <f t="shared" si="18"/>
         <v>0.29166666666666669</v>
       </c>
       <c r="P23" s="11">
-        <f>H23/H$3</f>
+        <f t="shared" si="19"/>
         <v>0.11874999999999999</v>
       </c>
       <c r="Q23" s="12">
-        <f>I23/I$3</f>
+        <f t="shared" si="20"/>
         <v>0.17989417989417988</v>
       </c>
       <c r="R23" s="15">
-        <f>SUM(B23:I23)</f>
+        <f t="shared" si="21"/>
         <v>78</v>
       </c>
     </row>
@@ -4189,7 +4189,7 @@
         <v>0</v>
       </c>
       <c r="G24" s="6">
-        <f>SUM(E24:F24)</f>
+        <f t="shared" si="12"/>
         <v>3</v>
       </c>
       <c r="H24" s="6">
@@ -4199,39 +4199,39 @@
         <v>41</v>
       </c>
       <c r="J24" s="11">
-        <f>B24/B$3</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="K24" s="11">
-        <f>C24/C$3</f>
+        <f t="shared" si="14"/>
         <v>0.1111111111111111</v>
       </c>
       <c r="L24" s="11">
-        <f>D24/D$3</f>
+        <f t="shared" si="15"/>
         <v>0.13513513513513514</v>
       </c>
       <c r="M24" s="11">
-        <f>E24/E$3</f>
+        <f t="shared" si="16"/>
         <v>0.23076923076923078</v>
       </c>
       <c r="N24" s="11">
-        <f>F24/F$3</f>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="O24" s="11">
-        <f>G24/G$3</f>
+        <f t="shared" si="18"/>
         <v>0.125</v>
       </c>
       <c r="P24" s="11">
-        <f>H24/H$3</f>
+        <f t="shared" si="19"/>
         <v>7.4999999999999997E-2</v>
       </c>
       <c r="Q24" s="12">
-        <f>I24/I$3</f>
+        <f t="shared" si="20"/>
         <v>0.21693121693121692</v>
       </c>
       <c r="R24" s="15">
-        <f>SUM(B24:I24)</f>
+        <f t="shared" si="21"/>
         <v>76</v>
       </c>
     </row>
@@ -4255,7 +4255,7 @@
         <v>1</v>
       </c>
       <c r="G25" s="6">
-        <f>SUM(E25:F25)</f>
+        <f t="shared" si="12"/>
         <v>2</v>
       </c>
       <c r="H25" s="6">
@@ -4265,39 +4265,39 @@
         <v>4</v>
       </c>
       <c r="J25" s="11">
-        <f>B25/B$3</f>
+        <f t="shared" si="13"/>
         <v>0.8928571428571429</v>
       </c>
       <c r="K25" s="11">
-        <f>C25/C$3</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="L25" s="11">
-        <f>D25/D$3</f>
+        <f t="shared" si="15"/>
         <v>2.7027027027027029E-2</v>
       </c>
       <c r="M25" s="11">
-        <f>E25/E$3</f>
+        <f t="shared" si="16"/>
         <v>7.6923076923076927E-2</v>
       </c>
       <c r="N25" s="11">
-        <f>F25/F$3</f>
+        <f t="shared" si="17"/>
         <v>9.0909090909090912E-2</v>
       </c>
       <c r="O25" s="11">
-        <f>G25/G$3</f>
+        <f t="shared" si="18"/>
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="P25" s="11">
-        <f>H25/H$3</f>
+        <f t="shared" si="19"/>
         <v>0.24374999999999999</v>
       </c>
       <c r="Q25" s="12">
-        <f>I25/I$3</f>
+        <f t="shared" si="20"/>
         <v>2.1164021164021163E-2</v>
       </c>
       <c r="R25" s="15">
-        <f>SUM(B25:I25)</f>
+        <f t="shared" si="21"/>
         <v>74</v>
       </c>
     </row>
@@ -4321,7 +4321,7 @@
         <v>3</v>
       </c>
       <c r="G26" s="6">
-        <f>SUM(E26:F26)</f>
+        <f t="shared" si="12"/>
         <v>6</v>
       </c>
       <c r="H26" s="6">
@@ -4331,39 +4331,39 @@
         <v>27</v>
       </c>
       <c r="J26" s="11">
-        <f>B26/B$3</f>
+        <f t="shared" si="13"/>
         <v>7.1428571428571425E-2</v>
       </c>
       <c r="K26" s="11">
-        <f>C26/C$3</f>
+        <f t="shared" si="14"/>
         <v>0.12698412698412698</v>
       </c>
       <c r="L26" s="11">
-        <f>D26/D$3</f>
+        <f t="shared" si="15"/>
         <v>2.7027027027027029E-2</v>
       </c>
       <c r="M26" s="11">
-        <f>E26/E$3</f>
+        <f t="shared" si="16"/>
         <v>0.23076923076923078</v>
       </c>
       <c r="N26" s="11">
-        <f>F26/F$3</f>
+        <f t="shared" si="17"/>
         <v>0.27272727272727271</v>
       </c>
       <c r="O26" s="11">
-        <f>G26/G$3</f>
+        <f t="shared" si="18"/>
         <v>0.25</v>
       </c>
       <c r="P26" s="11">
-        <f>H26/H$3</f>
+        <f t="shared" si="19"/>
         <v>0.10625</v>
       </c>
       <c r="Q26" s="12">
-        <f>I26/I$3</f>
+        <f t="shared" si="20"/>
         <v>0.14285714285714285</v>
       </c>
       <c r="R26" s="15">
-        <f>SUM(B26:I26)</f>
+        <f t="shared" si="21"/>
         <v>68</v>
       </c>
     </row>
@@ -4387,7 +4387,7 @@
         <v>0</v>
       </c>
       <c r="G27" s="6">
-        <f>SUM(E27:F27)</f>
+        <f t="shared" si="12"/>
         <v>2</v>
       </c>
       <c r="H27" s="6">
@@ -4397,39 +4397,39 @@
         <v>35</v>
       </c>
       <c r="J27" s="11">
-        <f>B27/B$3</f>
+        <f t="shared" si="13"/>
         <v>7.1428571428571425E-2</v>
       </c>
       <c r="K27" s="11">
-        <f>C27/C$3</f>
+        <f t="shared" si="14"/>
         <v>7.9365079365079361E-2</v>
       </c>
       <c r="L27" s="11">
-        <f>D27/D$3</f>
+        <f t="shared" si="15"/>
         <v>1.3513513513513514E-2</v>
       </c>
       <c r="M27" s="11">
-        <f>E27/E$3</f>
+        <f t="shared" si="16"/>
         <v>0.15384615384615385</v>
       </c>
       <c r="N27" s="11">
-        <f>F27/F$3</f>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="O27" s="11">
-        <f>G27/G$3</f>
+        <f t="shared" si="18"/>
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="P27" s="11">
-        <f>H27/H$3</f>
+        <f t="shared" si="19"/>
         <v>5.6250000000000001E-2</v>
       </c>
       <c r="Q27" s="12">
-        <f>I27/I$3</f>
+        <f t="shared" si="20"/>
         <v>0.18518518518518517</v>
       </c>
       <c r="R27" s="15">
-        <f>SUM(B27:I27)</f>
+        <f t="shared" si="21"/>
         <v>56</v>
       </c>
     </row>
@@ -4453,7 +4453,7 @@
         <v>0</v>
       </c>
       <c r="G28" s="6">
-        <f>SUM(E28:F28)</f>
+        <f t="shared" si="12"/>
         <v>2</v>
       </c>
       <c r="H28" s="6">
@@ -4463,39 +4463,39 @@
         <v>2</v>
       </c>
       <c r="J28" s="11">
-        <f>B28/B$3</f>
+        <f t="shared" si="13"/>
         <v>0.8214285714285714</v>
       </c>
       <c r="K28" s="11">
-        <f>C28/C$3</f>
+        <f t="shared" si="14"/>
         <v>1.5873015873015872E-2</v>
       </c>
       <c r="L28" s="11">
-        <f>D28/D$3</f>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="M28" s="11">
-        <f>E28/E$3</f>
+        <f t="shared" si="16"/>
         <v>0.15384615384615385</v>
       </c>
       <c r="N28" s="11">
-        <f>F28/F$3</f>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="O28" s="11">
-        <f>G28/G$3</f>
+        <f t="shared" si="18"/>
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="P28" s="11">
-        <f>H28/H$3</f>
+        <f t="shared" si="19"/>
         <v>3.7499999999999999E-2</v>
       </c>
       <c r="Q28" s="12">
-        <f>I28/I$3</f>
+        <f t="shared" si="20"/>
         <v>1.0582010582010581E-2</v>
       </c>
       <c r="R28" s="15">
-        <f>SUM(B28:I28)</f>
+        <f t="shared" si="21"/>
         <v>36</v>
       </c>
     </row>
@@ -4519,7 +4519,7 @@
         <v>0</v>
       </c>
       <c r="G29" s="6">
-        <f>SUM(E29:F29)</f>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
       <c r="H29" s="6">
@@ -4529,39 +4529,39 @@
         <v>20</v>
       </c>
       <c r="J29" s="11">
-        <f>B29/B$3</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="K29" s="11">
-        <f>C29/C$3</f>
+        <f t="shared" si="14"/>
         <v>6.3492063492063489E-2</v>
       </c>
       <c r="L29" s="11">
-        <f>D29/D$3</f>
+        <f t="shared" si="15"/>
         <v>1.3513513513513514E-2</v>
       </c>
       <c r="M29" s="11">
-        <f>E29/E$3</f>
+        <f t="shared" si="16"/>
         <v>7.6923076923076927E-2</v>
       </c>
       <c r="N29" s="11">
-        <f>F29/F$3</f>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="O29" s="11">
-        <f>G29/G$3</f>
+        <f t="shared" si="18"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="P29" s="11">
-        <f>H29/H$3</f>
+        <f t="shared" si="19"/>
         <v>1.2500000000000001E-2</v>
       </c>
       <c r="Q29" s="12">
-        <f>I29/I$3</f>
+        <f t="shared" si="20"/>
         <v>0.10582010582010581</v>
       </c>
       <c r="R29" s="15">
-        <f>SUM(B29:I29)</f>
+        <f t="shared" si="21"/>
         <v>29</v>
       </c>
     </row>
@@ -4585,7 +4585,7 @@
         <v>2</v>
       </c>
       <c r="G30" s="6">
-        <f>SUM(E30:F30)</f>
+        <f t="shared" si="12"/>
         <v>3</v>
       </c>
       <c r="H30" s="6">
@@ -4595,39 +4595,39 @@
         <v>9</v>
       </c>
       <c r="J30" s="11">
-        <f>B30/B$3</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="K30" s="11">
-        <f>C30/C$3</f>
+        <f t="shared" si="14"/>
         <v>6.3492063492063489E-2</v>
       </c>
       <c r="L30" s="11">
-        <f>D30/D$3</f>
+        <f t="shared" si="15"/>
         <v>1.3513513513513514E-2</v>
       </c>
       <c r="M30" s="11">
-        <f>E30/E$3</f>
+        <f t="shared" si="16"/>
         <v>7.6923076923076927E-2</v>
       </c>
       <c r="N30" s="11">
-        <f>F30/F$3</f>
+        <f t="shared" si="17"/>
         <v>0.18181818181818182</v>
       </c>
       <c r="O30" s="11">
-        <f>G30/G$3</f>
+        <f t="shared" si="18"/>
         <v>0.125</v>
       </c>
       <c r="P30" s="11">
-        <f>H30/H$3</f>
+        <f t="shared" si="19"/>
         <v>3.7499999999999999E-2</v>
       </c>
       <c r="Q30" s="12">
-        <f>I30/I$3</f>
+        <f t="shared" si="20"/>
         <v>4.7619047619047616E-2</v>
       </c>
       <c r="R30" s="15">
-        <f>SUM(B30:I30)</f>
+        <f t="shared" si="21"/>
         <v>26</v>
       </c>
     </row>
@@ -4651,7 +4651,7 @@
         <v>0</v>
       </c>
       <c r="G31" s="6">
-        <f>SUM(E31:F31)</f>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
       <c r="H31" s="6">
@@ -4661,39 +4661,39 @@
         <v>17</v>
       </c>
       <c r="J31" s="11">
-        <f>B31/B$3</f>
+        <f t="shared" si="13"/>
         <v>3.5714285714285712E-2</v>
       </c>
       <c r="K31" s="11">
-        <f>C31/C$3</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="L31" s="11">
-        <f>D31/D$3</f>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="M31" s="11">
-        <f>E31/E$3</f>
+        <f t="shared" si="16"/>
         <v>7.6923076923076927E-2</v>
       </c>
       <c r="N31" s="11">
-        <f>F31/F$3</f>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="O31" s="11">
-        <f>G31/G$3</f>
+        <f t="shared" si="18"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="P31" s="11">
-        <f>H31/H$3</f>
+        <f t="shared" si="19"/>
         <v>3.125E-2</v>
       </c>
       <c r="Q31" s="12">
-        <f>I31/I$3</f>
+        <f t="shared" si="20"/>
         <v>8.9947089947089942E-2</v>
       </c>
       <c r="R31" s="15">
-        <f>SUM(B31:I31)</f>
+        <f t="shared" si="21"/>
         <v>25</v>
       </c>
     </row>
@@ -4717,7 +4717,7 @@
         <v>0</v>
       </c>
       <c r="G32" s="6">
-        <f>SUM(E32:F32)</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="H32" s="6">
@@ -4727,39 +4727,39 @@
         <v>0</v>
       </c>
       <c r="J32" s="11">
-        <f>B32/B$3</f>
+        <f t="shared" si="13"/>
         <v>7.1428571428571425E-2</v>
       </c>
       <c r="K32" s="11">
-        <f>C32/C$3</f>
+        <f t="shared" si="14"/>
         <v>0.31746031746031744</v>
       </c>
       <c r="L32" s="11">
-        <f>D32/D$3</f>
+        <f t="shared" si="15"/>
         <v>2.7027027027027029E-2</v>
       </c>
       <c r="M32" s="11">
-        <f>E32/E$3</f>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="N32" s="11">
-        <f>F32/F$3</f>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="O32" s="11">
-        <f>G32/G$3</f>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="P32" s="11">
-        <f>H32/H$3</f>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="Q32" s="12">
-        <f>I32/I$3</f>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="R32" s="15">
-        <f>SUM(B32:I32)</f>
+        <f t="shared" si="21"/>
         <v>24</v>
       </c>
     </row>
@@ -4783,7 +4783,7 @@
         <v>0</v>
       </c>
       <c r="G33" s="6">
-        <f>SUM(E33:F33)</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="H33" s="6">
@@ -4793,39 +4793,39 @@
         <v>2</v>
       </c>
       <c r="J33" s="11">
-        <f>B33/B$3</f>
+        <f t="shared" si="13"/>
         <v>0.10714285714285714</v>
       </c>
       <c r="K33" s="11">
-        <f>C33/C$3</f>
+        <f t="shared" si="14"/>
         <v>0.15873015873015872</v>
       </c>
       <c r="L33" s="11">
-        <f>D33/D$3</f>
+        <f t="shared" si="15"/>
         <v>1.3513513513513514E-2</v>
       </c>
       <c r="M33" s="11">
-        <f>E33/E$3</f>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="N33" s="11">
-        <f>F33/F$3</f>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="O33" s="11">
-        <f>G33/G$3</f>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="P33" s="11">
-        <f>H33/H$3</f>
+        <f t="shared" si="19"/>
         <v>1.8749999999999999E-2</v>
       </c>
       <c r="Q33" s="12">
-        <f>I33/I$3</f>
+        <f t="shared" si="20"/>
         <v>1.0582010582010581E-2</v>
       </c>
       <c r="R33" s="15">
-        <f>SUM(B33:I33)</f>
+        <f t="shared" si="21"/>
         <v>19</v>
       </c>
     </row>
@@ -4849,7 +4849,7 @@
         <v>1</v>
       </c>
       <c r="G34" s="6">
-        <f>SUM(E34:F34)</f>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
       <c r="H34" s="6">
@@ -4859,39 +4859,39 @@
         <v>4</v>
       </c>
       <c r="J34" s="11">
-        <f>B34/B$3</f>
+        <f t="shared" si="13"/>
         <v>7.1428571428571425E-2</v>
       </c>
       <c r="K34" s="11">
-        <f>C34/C$3</f>
+        <f t="shared" si="14"/>
         <v>6.3492063492063489E-2</v>
       </c>
       <c r="L34" s="11">
-        <f>D34/D$3</f>
+        <f t="shared" si="15"/>
         <v>4.0540540540540543E-2</v>
       </c>
       <c r="M34" s="11">
-        <f>E34/E$3</f>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="N34" s="11">
-        <f>F34/F$3</f>
+        <f t="shared" si="17"/>
         <v>9.0909090909090912E-2</v>
       </c>
       <c r="O34" s="11">
-        <f>G34/G$3</f>
+        <f t="shared" si="18"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="P34" s="11">
-        <f>H34/H$3</f>
+        <f t="shared" si="19"/>
         <v>6.2500000000000003E-3</v>
       </c>
       <c r="Q34" s="12">
-        <f>I34/I$3</f>
+        <f t="shared" si="20"/>
         <v>2.1164021164021163E-2</v>
       </c>
       <c r="R34" s="15">
-        <f>SUM(B34:I34)</f>
+        <f t="shared" si="21"/>
         <v>16</v>
       </c>
     </row>
@@ -4915,7 +4915,7 @@
         <v>0</v>
       </c>
       <c r="G35" s="6">
-        <f>SUM(E35:F35)</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="H35" s="6">
@@ -4925,39 +4925,39 @@
         <v>2</v>
       </c>
       <c r="J35" s="11">
-        <f>B35/B$3</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="K35" s="11">
-        <f>C35/C$3</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="L35" s="11">
-        <f>D35/D$3</f>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="M35" s="11">
-        <f>E35/E$3</f>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="N35" s="11">
-        <f>F35/F$3</f>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="O35" s="11">
-        <f>G35/G$3</f>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="P35" s="11">
-        <f>H35/H$3</f>
+        <f t="shared" si="19"/>
         <v>5.6250000000000001E-2</v>
       </c>
       <c r="Q35" s="12">
-        <f>I35/I$3</f>
+        <f t="shared" si="20"/>
         <v>1.0582010582010581E-2</v>
       </c>
       <c r="R35" s="15">
-        <f>SUM(B35:I35)</f>
+        <f t="shared" si="21"/>
         <v>11</v>
       </c>
     </row>
@@ -4981,7 +4981,7 @@
         <v>0</v>
       </c>
       <c r="G36" s="6">
-        <f>SUM(E36:F36)</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="H36" s="6">
@@ -4991,39 +4991,39 @@
         <v>6</v>
       </c>
       <c r="J36" s="11">
-        <f>B36/B$3</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="K36" s="11">
-        <f>C36/C$3</f>
+        <f t="shared" si="14"/>
         <v>3.1746031746031744E-2</v>
       </c>
       <c r="L36" s="11">
-        <f>D36/D$3</f>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="M36" s="11">
-        <f>E36/E$3</f>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="N36" s="11">
-        <f>F36/F$3</f>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="O36" s="11">
-        <f>G36/G$3</f>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="P36" s="11">
-        <f>H36/H$3</f>
+        <f t="shared" si="19"/>
         <v>1.8749999999999999E-2</v>
       </c>
       <c r="Q36" s="12">
-        <f>I36/I$3</f>
+        <f t="shared" si="20"/>
         <v>3.1746031746031744E-2</v>
       </c>
       <c r="R36" s="15">
-        <f>SUM(B36:I36)</f>
+        <f t="shared" si="21"/>
         <v>11</v>
       </c>
     </row>
@@ -5047,7 +5047,7 @@
         <v>0</v>
       </c>
       <c r="G37" s="6">
-        <f>SUM(E37:F37)</f>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
       <c r="H37" s="6">
@@ -5057,39 +5057,39 @@
         <v>5</v>
       </c>
       <c r="J37" s="11">
-        <f>B37/B$3</f>
+        <f t="shared" ref="J37:J58" si="22">B37/B$3</f>
         <v>0</v>
       </c>
       <c r="K37" s="11">
-        <f>C37/C$3</f>
+        <f t="shared" ref="K37:K58" si="23">C37/C$3</f>
         <v>4.7619047619047616E-2</v>
       </c>
       <c r="L37" s="11">
-        <f>D37/D$3</f>
+        <f t="shared" ref="L37:L58" si="24">D37/D$3</f>
         <v>0</v>
       </c>
       <c r="M37" s="11">
-        <f>E37/E$3</f>
+        <f t="shared" ref="M37:M58" si="25">E37/E$3</f>
         <v>7.6923076923076927E-2</v>
       </c>
       <c r="N37" s="11">
-        <f>F37/F$3</f>
+        <f t="shared" ref="N37:N58" si="26">F37/F$3</f>
         <v>0</v>
       </c>
       <c r="O37" s="11">
-        <f>G37/G$3</f>
+        <f t="shared" ref="O37:O58" si="27">G37/G$3</f>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="P37" s="11">
-        <f>H37/H$3</f>
+        <f t="shared" ref="P37:P58" si="28">H37/H$3</f>
         <v>0</v>
       </c>
       <c r="Q37" s="12">
-        <f>I37/I$3</f>
+        <f t="shared" ref="Q37:Q58" si="29">I37/I$3</f>
         <v>2.6455026455026454E-2</v>
       </c>
       <c r="R37" s="15">
-        <f>SUM(B37:I37)</f>
+        <f t="shared" ref="R37:R58" si="30">SUM(B37:I37)</f>
         <v>10</v>
       </c>
     </row>
@@ -5113,7 +5113,7 @@
         <v>0</v>
       </c>
       <c r="G38" s="6">
-        <f>SUM(E38:F38)</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="H38" s="6">
@@ -5123,39 +5123,39 @@
         <v>0</v>
       </c>
       <c r="J38" s="11">
-        <f>B38/B$3</f>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="K38" s="11">
-        <f>C38/C$3</f>
+        <f t="shared" si="23"/>
         <v>6.3492063492063489E-2</v>
       </c>
       <c r="L38" s="11">
-        <f>D38/D$3</f>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="M38" s="11">
-        <f>E38/E$3</f>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="N38" s="11">
-        <f>F38/F$3</f>
+        <f t="shared" si="26"/>
         <v>0</v>
       </c>
       <c r="O38" s="11">
-        <f>G38/G$3</f>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="P38" s="11">
-        <f>H38/H$3</f>
+        <f t="shared" si="28"/>
         <v>3.7499999999999999E-2</v>
       </c>
       <c r="Q38" s="12">
-        <f>I38/I$3</f>
+        <f t="shared" si="29"/>
         <v>0</v>
       </c>
       <c r="R38" s="15">
-        <f>SUM(B38:I38)</f>
+        <f t="shared" si="30"/>
         <v>10</v>
       </c>
     </row>
@@ -5179,7 +5179,7 @@
         <v>0</v>
       </c>
       <c r="G39" s="6">
-        <f>SUM(E39:F39)</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="H39" s="6">
@@ -5189,39 +5189,39 @@
         <v>0</v>
       </c>
       <c r="J39" s="11">
-        <f>B39/B$3</f>
+        <f t="shared" si="22"/>
         <v>0.21428571428571427</v>
       </c>
       <c r="K39" s="11">
-        <f>C39/C$3</f>
+        <f t="shared" si="23"/>
         <v>3.1746031746031744E-2</v>
       </c>
       <c r="L39" s="11">
-        <f>D39/D$3</f>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="M39" s="11">
-        <f>E39/E$3</f>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="N39" s="11">
-        <f>F39/F$3</f>
+        <f t="shared" si="26"/>
         <v>0</v>
       </c>
       <c r="O39" s="11">
-        <f>G39/G$3</f>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="P39" s="11">
-        <f>H39/H$3</f>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="Q39" s="12">
-        <f>I39/I$3</f>
+        <f t="shared" si="29"/>
         <v>0</v>
       </c>
       <c r="R39" s="15">
-        <f>SUM(B39:I39)</f>
+        <f t="shared" si="30"/>
         <v>8</v>
       </c>
     </row>
@@ -5245,7 +5245,7 @@
         <v>1</v>
       </c>
       <c r="G40" s="6">
-        <f>SUM(E40:F40)</f>
+        <f t="shared" si="12"/>
         <v>2</v>
       </c>
       <c r="H40" s="6">
@@ -5255,39 +5255,39 @@
         <v>2</v>
       </c>
       <c r="J40" s="11">
-        <f>B40/B$3</f>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="K40" s="11">
-        <f>C40/C$3</f>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="L40" s="11">
-        <f>D40/D$3</f>
+        <f t="shared" si="24"/>
         <v>1.3513513513513514E-2</v>
       </c>
       <c r="M40" s="11">
-        <f>E40/E$3</f>
+        <f t="shared" si="25"/>
         <v>7.6923076923076927E-2</v>
       </c>
       <c r="N40" s="11">
-        <f>F40/F$3</f>
+        <f t="shared" si="26"/>
         <v>9.0909090909090912E-2</v>
       </c>
       <c r="O40" s="11">
-        <f>G40/G$3</f>
+        <f t="shared" si="27"/>
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="P40" s="11">
-        <f>H40/H$3</f>
+        <f t="shared" si="28"/>
         <v>6.2500000000000003E-3</v>
       </c>
       <c r="Q40" s="12">
-        <f>I40/I$3</f>
+        <f t="shared" si="29"/>
         <v>1.0582010582010581E-2</v>
       </c>
       <c r="R40" s="15">
-        <f>SUM(B40:I40)</f>
+        <f t="shared" si="30"/>
         <v>8</v>
       </c>
     </row>
@@ -5311,7 +5311,7 @@
         <v>1</v>
       </c>
       <c r="G41" s="6">
-        <f>SUM(E41:F41)</f>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
       <c r="H41" s="6">
@@ -5321,39 +5321,39 @@
         <v>0</v>
       </c>
       <c r="J41" s="11">
-        <f>B41/B$3</f>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="K41" s="11">
-        <f>C41/C$3</f>
+        <f t="shared" si="23"/>
         <v>9.5238095238095233E-2</v>
       </c>
       <c r="L41" s="11">
-        <f>D41/D$3</f>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="M41" s="11">
-        <f>E41/E$3</f>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="N41" s="11">
-        <f>F41/F$3</f>
+        <f t="shared" si="26"/>
         <v>9.0909090909090912E-2</v>
       </c>
       <c r="O41" s="11">
-        <f>G41/G$3</f>
+        <f t="shared" si="27"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="P41" s="11">
-        <f>H41/H$3</f>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="Q41" s="12">
-        <f>I41/I$3</f>
+        <f t="shared" si="29"/>
         <v>0</v>
       </c>
       <c r="R41" s="15">
-        <f>SUM(B41:I41)</f>
+        <f t="shared" si="30"/>
         <v>8</v>
       </c>
     </row>
@@ -5377,7 +5377,7 @@
         <v>1</v>
       </c>
       <c r="G42" s="6">
-        <f>SUM(E42:F42)</f>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
       <c r="H42" s="6">
@@ -5387,39 +5387,39 @@
         <v>0</v>
       </c>
       <c r="J42" s="11">
-        <f>B42/B$3</f>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="K42" s="11">
-        <f>C42/C$3</f>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="L42" s="11">
-        <f>D42/D$3</f>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="M42" s="11">
-        <f>E42/E$3</f>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="N42" s="11">
-        <f>F42/F$3</f>
+        <f t="shared" si="26"/>
         <v>9.0909090909090912E-2</v>
       </c>
       <c r="O42" s="11">
-        <f>G42/G$3</f>
+        <f t="shared" si="27"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="P42" s="11">
-        <f>H42/H$3</f>
+        <f t="shared" si="28"/>
         <v>1.8749999999999999E-2</v>
       </c>
       <c r="Q42" s="12">
-        <f>I42/I$3</f>
+        <f t="shared" si="29"/>
         <v>0</v>
       </c>
       <c r="R42" s="15">
-        <f>SUM(B42:I42)</f>
+        <f t="shared" si="30"/>
         <v>5</v>
       </c>
     </row>
@@ -5443,7 +5443,7 @@
         <v>0</v>
       </c>
       <c r="G43" s="36">
-        <f t="shared" ref="G6:G58" si="12">SUM(E43:F43)</f>
+        <f t="shared" ref="G43:G58" si="31">SUM(E43:F43)</f>
         <v>0</v>
       </c>
       <c r="H43" s="36">
@@ -5453,39 +5453,39 @@
         <v>4</v>
       </c>
       <c r="J43" s="39">
-        <f>B43/B$3</f>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="K43" s="39">
-        <f>C43/C$3</f>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="L43" s="39">
-        <f>D43/D$3</f>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="M43" s="39">
-        <f>E43/E$3</f>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="N43" s="39">
-        <f>F43/F$3</f>
+        <f t="shared" si="26"/>
         <v>0</v>
       </c>
       <c r="O43" s="39">
-        <f>G43/G$3</f>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="P43" s="39">
-        <f>H43/H$3</f>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="Q43" s="40">
-        <f>I43/I$3</f>
+        <f t="shared" si="29"/>
         <v>2.1164021164021163E-2</v>
       </c>
       <c r="R43" s="15">
-        <f>SUM(B43:I43)</f>
+        <f t="shared" si="30"/>
         <v>4</v>
       </c>
     </row>
@@ -5509,7 +5509,7 @@
         <v>0</v>
       </c>
       <c r="G44" s="6">
-        <f t="shared" si="12"/>
+        <f t="shared" si="31"/>
         <v>0</v>
       </c>
       <c r="H44" s="6">
@@ -5519,39 +5519,39 @@
         <v>0</v>
       </c>
       <c r="J44" s="11">
-        <f>B44/B$3</f>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="K44" s="11">
-        <f>C44/C$3</f>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="L44" s="11">
-        <f>D44/D$3</f>
+        <f t="shared" si="24"/>
         <v>4.0540540540540543E-2</v>
       </c>
       <c r="M44" s="11">
-        <f>E44/E$3</f>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="N44" s="11">
-        <f>F44/F$3</f>
+        <f t="shared" si="26"/>
         <v>0</v>
       </c>
       <c r="O44" s="11">
-        <f>G44/G$3</f>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="P44" s="11">
-        <f>H44/H$3</f>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="Q44" s="12">
-        <f>I44/I$3</f>
+        <f t="shared" si="29"/>
         <v>0</v>
       </c>
       <c r="R44" s="15">
-        <f>SUM(B44:I44)</f>
+        <f t="shared" si="30"/>
         <v>3</v>
       </c>
     </row>
@@ -5575,7 +5575,7 @@
         <v>0</v>
       </c>
       <c r="G45" s="6">
-        <f t="shared" si="12"/>
+        <f t="shared" si="31"/>
         <v>0</v>
       </c>
       <c r="H45" s="6">
@@ -5585,39 +5585,39 @@
         <v>0</v>
       </c>
       <c r="J45" s="11">
-        <f>B45/B$3</f>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="K45" s="11">
-        <f>C45/C$3</f>
+        <f t="shared" si="23"/>
         <v>4.7619047619047616E-2</v>
       </c>
       <c r="L45" s="11">
-        <f>D45/D$3</f>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="M45" s="11">
-        <f>E45/E$3</f>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="N45" s="11">
-        <f>F45/F$3</f>
+        <f t="shared" si="26"/>
         <v>0</v>
       </c>
       <c r="O45" s="11">
-        <f>G45/G$3</f>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="P45" s="11">
-        <f>H45/H$3</f>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="Q45" s="12">
-        <f>I45/I$3</f>
+        <f t="shared" si="29"/>
         <v>0</v>
       </c>
       <c r="R45" s="15">
-        <f>SUM(B45:I45)</f>
+        <f t="shared" si="30"/>
         <v>3</v>
       </c>
     </row>
@@ -5641,7 +5641,7 @@
         <v>0</v>
       </c>
       <c r="G46" s="6">
-        <f t="shared" si="12"/>
+        <f t="shared" si="31"/>
         <v>0</v>
       </c>
       <c r="H46" s="6">
@@ -5651,39 +5651,39 @@
         <v>3</v>
       </c>
       <c r="J46" s="11">
-        <f>B46/B$3</f>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="K46" s="11">
-        <f>C46/C$3</f>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="L46" s="11">
-        <f>D46/D$3</f>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="M46" s="11">
-        <f>E46/E$3</f>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="N46" s="11">
-        <f>F46/F$3</f>
+        <f t="shared" si="26"/>
         <v>0</v>
       </c>
       <c r="O46" s="11">
-        <f>G46/G$3</f>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="P46" s="11">
-        <f>H46/H$3</f>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="Q46" s="12">
-        <f>I46/I$3</f>
+        <f t="shared" si="29"/>
         <v>1.5873015873015872E-2</v>
       </c>
       <c r="R46" s="15">
-        <f>SUM(B46:I46)</f>
+        <f t="shared" si="30"/>
         <v>3</v>
       </c>
     </row>
@@ -5707,7 +5707,7 @@
         <v>0</v>
       </c>
       <c r="G47" s="6">
-        <f t="shared" si="12"/>
+        <f t="shared" si="31"/>
         <v>0</v>
       </c>
       <c r="H47" s="6">
@@ -5717,39 +5717,39 @@
         <v>1</v>
       </c>
       <c r="J47" s="11">
-        <f>B47/B$3</f>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="K47" s="11">
-        <f>C47/C$3</f>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="L47" s="11">
-        <f>D47/D$3</f>
+        <f t="shared" si="24"/>
         <v>1.3513513513513514E-2</v>
       </c>
       <c r="M47" s="11">
-        <f>E47/E$3</f>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="N47" s="11">
-        <f>F47/F$3</f>
+        <f t="shared" si="26"/>
         <v>0</v>
       </c>
       <c r="O47" s="11">
-        <f>G47/G$3</f>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="P47" s="11">
-        <f>H47/H$3</f>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="Q47" s="12">
-        <f>I47/I$3</f>
+        <f t="shared" si="29"/>
         <v>5.2910052910052907E-3</v>
       </c>
       <c r="R47" s="15">
-        <f>SUM(B47:I47)</f>
+        <f t="shared" si="30"/>
         <v>2</v>
       </c>
     </row>
@@ -5773,7 +5773,7 @@
         <v>0</v>
       </c>
       <c r="G48" s="6">
-        <f t="shared" si="12"/>
+        <f t="shared" si="31"/>
         <v>0</v>
       </c>
       <c r="H48" s="6">
@@ -5783,39 +5783,39 @@
         <v>0</v>
       </c>
       <c r="J48" s="11">
-        <f>B48/B$3</f>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="K48" s="11">
-        <f>C48/C$3</f>
+        <f t="shared" si="23"/>
         <v>3.1746031746031744E-2</v>
       </c>
       <c r="L48" s="11">
-        <f>D48/D$3</f>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="M48" s="11">
-        <f>E48/E$3</f>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="N48" s="11">
-        <f>F48/F$3</f>
+        <f t="shared" si="26"/>
         <v>0</v>
       </c>
       <c r="O48" s="11">
-        <f>G48/G$3</f>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="P48" s="11">
-        <f>H48/H$3</f>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="Q48" s="12">
-        <f>I48/I$3</f>
+        <f t="shared" si="29"/>
         <v>0</v>
       </c>
       <c r="R48" s="15">
-        <f>SUM(B48:I48)</f>
+        <f t="shared" si="30"/>
         <v>2</v>
       </c>
     </row>
@@ -5839,7 +5839,7 @@
         <v>0</v>
       </c>
       <c r="G49" s="6">
-        <f t="shared" si="12"/>
+        <f t="shared" si="31"/>
         <v>1</v>
       </c>
       <c r="H49" s="6">
@@ -5849,39 +5849,39 @@
         <v>0</v>
       </c>
       <c r="J49" s="11">
-        <f>B49/B$3</f>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="K49" s="11">
-        <f>C49/C$3</f>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="L49" s="11">
-        <f>D49/D$3</f>
+        <f t="shared" si="24"/>
         <v>1.3513513513513514E-2</v>
       </c>
       <c r="M49" s="11">
-        <f>E49/E$3</f>
+        <f t="shared" si="25"/>
         <v>7.6923076923076927E-2</v>
       </c>
       <c r="N49" s="11">
-        <f>F49/F$3</f>
+        <f t="shared" si="26"/>
         <v>0</v>
       </c>
       <c r="O49" s="11">
-        <f>G49/G$3</f>
+        <f t="shared" si="27"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="P49" s="11">
-        <f>H49/H$3</f>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="Q49" s="12">
-        <f>I49/I$3</f>
+        <f t="shared" si="29"/>
         <v>0</v>
       </c>
       <c r="R49" s="15">
-        <f>SUM(B49:I49)</f>
+        <f t="shared" si="30"/>
         <v>3</v>
       </c>
     </row>
@@ -5905,7 +5905,7 @@
         <v>0</v>
       </c>
       <c r="G50" s="6">
-        <f t="shared" si="12"/>
+        <f t="shared" si="31"/>
         <v>0</v>
       </c>
       <c r="H50" s="6">
@@ -5915,39 +5915,39 @@
         <v>0</v>
       </c>
       <c r="J50" s="11">
-        <f>B50/B$3</f>
+        <f t="shared" si="22"/>
         <v>3.5714285714285712E-2</v>
       </c>
       <c r="K50" s="11">
-        <f>C50/C$3</f>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="L50" s="11">
-        <f>D50/D$3</f>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="M50" s="11">
-        <f>E50/E$3</f>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="N50" s="11">
-        <f>F50/F$3</f>
+        <f t="shared" si="26"/>
         <v>0</v>
       </c>
       <c r="O50" s="11">
-        <f>G50/G$3</f>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="P50" s="11">
-        <f>H50/H$3</f>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="Q50" s="12">
-        <f>I50/I$3</f>
+        <f t="shared" si="29"/>
         <v>0</v>
       </c>
       <c r="R50" s="15">
-        <f>SUM(B50:I50)</f>
+        <f t="shared" si="30"/>
         <v>1</v>
       </c>
     </row>
@@ -5971,7 +5971,7 @@
         <v>0</v>
       </c>
       <c r="G51" s="6">
-        <f t="shared" si="12"/>
+        <f t="shared" si="31"/>
         <v>0</v>
       </c>
       <c r="H51" s="6">
@@ -5981,39 +5981,39 @@
         <v>0</v>
       </c>
       <c r="J51" s="11">
-        <f>B51/B$3</f>
+        <f t="shared" si="22"/>
         <v>3.5714285714285712E-2</v>
       </c>
       <c r="K51" s="11">
-        <f>C51/C$3</f>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="L51" s="11">
-        <f>D51/D$3</f>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="M51" s="11">
-        <f>E51/E$3</f>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="N51" s="11">
-        <f>F51/F$3</f>
+        <f t="shared" si="26"/>
         <v>0</v>
       </c>
       <c r="O51" s="11">
-        <f>G51/G$3</f>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="P51" s="11">
-        <f>H51/H$3</f>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="Q51" s="12">
-        <f>I51/I$3</f>
+        <f t="shared" si="29"/>
         <v>0</v>
       </c>
       <c r="R51" s="15">
-        <f>SUM(B51:I51)</f>
+        <f t="shared" si="30"/>
         <v>1</v>
       </c>
     </row>
@@ -6037,7 +6037,7 @@
         <v>0</v>
       </c>
       <c r="G52" s="6">
-        <f t="shared" si="12"/>
+        <f t="shared" si="31"/>
         <v>0</v>
       </c>
       <c r="H52" s="6">
@@ -6047,39 +6047,39 @@
         <v>0</v>
       </c>
       <c r="J52" s="11">
-        <f>B52/B$3</f>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="K52" s="11">
-        <f>C52/C$3</f>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="L52" s="11">
-        <f>D52/D$3</f>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="M52" s="11">
-        <f>E52/E$3</f>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="N52" s="11">
-        <f>F52/F$3</f>
+        <f t="shared" si="26"/>
         <v>0</v>
       </c>
       <c r="O52" s="11">
-        <f>G52/G$3</f>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="P52" s="11">
-        <f>H52/H$3</f>
+        <f t="shared" si="28"/>
         <v>6.2500000000000003E-3</v>
       </c>
       <c r="Q52" s="12">
-        <f>I52/I$3</f>
+        <f t="shared" si="29"/>
         <v>0</v>
       </c>
       <c r="R52" s="15">
-        <f>SUM(B52:I52)</f>
+        <f t="shared" si="30"/>
         <v>1</v>
       </c>
     </row>
@@ -6103,7 +6103,7 @@
         <v>0</v>
       </c>
       <c r="G53" s="6">
-        <f t="shared" si="12"/>
+        <f t="shared" si="31"/>
         <v>0</v>
       </c>
       <c r="H53" s="6">
@@ -6113,39 +6113,39 @@
         <v>1</v>
       </c>
       <c r="J53" s="11">
-        <f>B53/B$3</f>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="K53" s="11">
-        <f>C53/C$3</f>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="L53" s="11">
-        <f>D53/D$3</f>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="M53" s="11">
-        <f>E53/E$3</f>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="N53" s="11">
-        <f>F53/F$3</f>
+        <f t="shared" si="26"/>
         <v>0</v>
       </c>
       <c r="O53" s="11">
-        <f>G53/G$3</f>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="P53" s="11">
-        <f>H53/H$3</f>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="Q53" s="12">
-        <f>I53/I$3</f>
+        <f t="shared" si="29"/>
         <v>5.2910052910052907E-3</v>
       </c>
       <c r="R53" s="15">
-        <f>SUM(B53:I53)</f>
+        <f t="shared" si="30"/>
         <v>1</v>
       </c>
     </row>
@@ -6169,7 +6169,7 @@
         <v>0</v>
       </c>
       <c r="G54" s="6">
-        <f t="shared" si="12"/>
+        <f t="shared" si="31"/>
         <v>0</v>
       </c>
       <c r="H54" s="6">
@@ -6179,39 +6179,39 @@
         <v>0</v>
       </c>
       <c r="J54" s="11">
-        <f>B54/B$3</f>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="K54" s="11">
-        <f>C54/C$3</f>
+        <f t="shared" si="23"/>
         <v>1.5873015873015872E-2</v>
       </c>
       <c r="L54" s="11">
-        <f>D54/D$3</f>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="M54" s="11">
-        <f>E54/E$3</f>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="N54" s="11">
-        <f>F54/F$3</f>
+        <f t="shared" si="26"/>
         <v>0</v>
       </c>
       <c r="O54" s="11">
-        <f>G54/G$3</f>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="P54" s="11">
-        <f>H54/H$3</f>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="Q54" s="12">
-        <f>I54/I$3</f>
+        <f t="shared" si="29"/>
         <v>0</v>
       </c>
       <c r="R54" s="15">
-        <f>SUM(B54:I54)</f>
+        <f t="shared" si="30"/>
         <v>1</v>
       </c>
     </row>
@@ -6235,7 +6235,7 @@
         <v>0</v>
       </c>
       <c r="G55" s="6">
-        <f t="shared" si="12"/>
+        <f t="shared" si="31"/>
         <v>0</v>
       </c>
       <c r="H55" s="6">
@@ -6245,39 +6245,39 @@
         <v>0</v>
       </c>
       <c r="J55" s="11">
-        <f>B55/B$3</f>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="K55" s="11">
-        <f>C55/C$3</f>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="L55" s="11">
-        <f>D55/D$3</f>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="M55" s="11">
-        <f>E55/E$3</f>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="N55" s="11">
-        <f>F55/F$3</f>
+        <f t="shared" si="26"/>
         <v>0</v>
       </c>
       <c r="O55" s="11">
-        <f>G55/G$3</f>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="P55" s="11">
-        <f>H55/H$3</f>
+        <f t="shared" si="28"/>
         <v>6.2500000000000003E-3</v>
       </c>
       <c r="Q55" s="12">
-        <f>I55/I$3</f>
+        <f t="shared" si="29"/>
         <v>0</v>
       </c>
       <c r="R55" s="15">
-        <f>SUM(B55:I55)</f>
+        <f t="shared" si="30"/>
         <v>1</v>
       </c>
     </row>
@@ -6301,7 +6301,7 @@
         <v>0</v>
       </c>
       <c r="G56" s="6">
-        <f t="shared" si="12"/>
+        <f t="shared" si="31"/>
         <v>0</v>
       </c>
       <c r="H56" s="6">
@@ -6311,39 +6311,39 @@
         <v>0</v>
       </c>
       <c r="J56" s="11">
-        <f>B56/B$3</f>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="K56" s="11">
-        <f>C56/C$3</f>
+        <f t="shared" si="23"/>
         <v>1.5873015873015872E-2</v>
       </c>
       <c r="L56" s="11">
-        <f>D56/D$3</f>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="M56" s="11">
-        <f>E56/E$3</f>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="N56" s="11">
-        <f>F56/F$3</f>
+        <f t="shared" si="26"/>
         <v>0</v>
       </c>
       <c r="O56" s="11">
-        <f>G56/G$3</f>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="P56" s="11">
-        <f>H56/H$3</f>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="Q56" s="12">
-        <f>I56/I$3</f>
+        <f t="shared" si="29"/>
         <v>0</v>
       </c>
       <c r="R56" s="15">
-        <f>SUM(B56:I56)</f>
+        <f t="shared" si="30"/>
         <v>1</v>
       </c>
     </row>
@@ -6367,7 +6367,7 @@
         <v>0</v>
       </c>
       <c r="G57" s="6">
-        <f t="shared" si="12"/>
+        <f t="shared" si="31"/>
         <v>0</v>
       </c>
       <c r="H57" s="6">
@@ -6377,39 +6377,39 @@
         <v>0</v>
       </c>
       <c r="J57" s="11">
-        <f>B57/B$3</f>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="K57" s="11">
-        <f>C57/C$3</f>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="L57" s="11">
-        <f>D57/D$3</f>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="M57" s="11">
-        <f>E57/E$3</f>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="N57" s="11">
-        <f>F57/F$3</f>
+        <f t="shared" si="26"/>
         <v>0</v>
       </c>
       <c r="O57" s="11">
-        <f>G57/G$3</f>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="P57" s="11">
-        <f>H57/H$3</f>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="Q57" s="12">
-        <f>I57/I$3</f>
+        <f t="shared" si="29"/>
         <v>0</v>
       </c>
       <c r="R57" s="15">
-        <f>SUM(B57:I57)</f>
+        <f t="shared" si="30"/>
         <v>0</v>
       </c>
     </row>
@@ -6433,7 +6433,7 @@
         <v>0</v>
       </c>
       <c r="G58" s="9">
-        <f t="shared" si="12"/>
+        <f t="shared" si="31"/>
         <v>0</v>
       </c>
       <c r="H58" s="9">
@@ -6443,39 +6443,39 @@
         <v>0</v>
       </c>
       <c r="J58" s="13">
-        <f>B58/B$3</f>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="K58" s="13">
-        <f>C58/C$3</f>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="L58" s="13">
-        <f>D58/D$3</f>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="M58" s="13">
-        <f>E58/E$3</f>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="N58" s="13">
-        <f>F58/F$3</f>
+        <f t="shared" si="26"/>
         <v>0</v>
       </c>
       <c r="O58" s="13">
-        <f>G58/G$3</f>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="P58" s="13">
-        <f>H58/H$3</f>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="Q58" s="14">
-        <f>I58/I$3</f>
+        <f t="shared" si="29"/>
         <v>0</v>
       </c>
       <c r="R58" s="15">
-        <f>SUM(B58:I58)</f>
+        <f t="shared" si="30"/>
         <v>0</v>
       </c>
     </row>
@@ -6886,7 +6886,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <ignoredErrors>
-    <ignoredError sqref="G43:G58 G3" formulaRange="1"/>
+    <ignoredError sqref="G43:G58 G3 G5:G42" formulaRange="1"/>
     <ignoredError sqref="G4" formula="1" formulaRange="1"/>
   </ignoredErrors>
 </worksheet>

</xml_diff>